<commit_message>
cargas csv MS e Capacitação FHIR
</commit_message>
<xml_diff>
--- a/Entregaveis/Entrega_1_RepositorioSemantico/Imunizacao/ViadeAdministracaoPNI.xlsx
+++ b/Entregaveis/Entrega_1_RepositorioSemantico/Imunizacao/ViadeAdministracaoPNI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Entregaveis/Entrega_1_RepositorioSemantico/Imunizacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93514F30-0BB1-5B4D-AE97-EF12224C7A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1142C5D-F89C-A245-8EE7-0BEB9BB319F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{08882ECF-919B-774E-915F-DE7A900954DF}"/>
   </bookViews>
@@ -84,10 +84,12 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
-      <name val="Helvetica Neue"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,15 +109,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,12 +435,12 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,6 +492,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{E95D87F9-145C-E649-B0BA-5188E8963F05}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>